<commit_message>
qc_rules as of Apr. 17
</commit_message>
<xml_diff>
--- a/qc_rules_recruitment.xlsx
+++ b/qc_rules_recruitment.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersjm/Documents/qaqc_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1B485E-0BC5-CF47-89F8-3F4AC870EDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D54C8-968A-AC40-9C0E-F6A2A6887CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="500" windowWidth="30240" windowHeight="17780" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
+    <workbookView xWindow="-37580" yWindow="-3480" windowWidth="35920" windowHeight="17780" activeTab="6" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
   </bookViews>
   <sheets>
-    <sheet name="QAQC_staged" sheetId="7" r:id="rId1"/>
-    <sheet name="QAQC" sheetId="1" r:id="rId2"/>
+    <sheet name="QAQC" sheetId="1" r:id="rId1"/>
+    <sheet name="on_deck" sheetId="7" r:id="rId2"/>
     <sheet name="Payment Rules" sheetId="6" r:id="rId3"/>
     <sheet name="Refusal_Withdrawel" sheetId="2" r:id="rId4"/>
     <sheet name="qctype descriptions" sheetId="3" r:id="rId5"/>
@@ -254,8 +254,35 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2BE77726-DB08-3448-8230-B667FCA9D175}</author>
+    <author>tc={13F41FFA-F201-0240-B037-1C67A50FB39B}</author>
+  </authors>
+  <commentList>
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{2BE77726-DB08-3448-8230-B667FCA9D175}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Need to add a crossvaligdation option for checking if the cross variable is a valid date in order to execute this rule</t>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="1" shapeId="0" xr:uid="{13F41FFA-F201-0240-B037-1C67A50FB39B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    These ones need a tweak to the code. “crossValid1 is not populated” rule should not flag participants for whom the ConceptID of interest is empty.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="578">
   <si>
     <t>Label</t>
   </si>
@@ -1983,34 +2010,19 @@
     <t>If user profile submitted (d_d_699625233) = yes (353358909) then consented (d_919254129) = yes (353358909)</t>
   </si>
   <si>
-    <t>If verification status (d_821247024) = verified, cannot be verified, or duplicate (197316935, 219863910, 922622075) then sign in (d_230663853) = yes (353358909)</t>
-  </si>
-  <si>
-    <t>If verification status (d_821247024) = verified, cannot be verified, or duplicate (197316935, 219863910, 922622075) then consented (d_919254129) = yes (353358909)</t>
-  </si>
-  <si>
-    <t>If verification status (d_821247024) = verified, cannot be verified, or duplicate (197316935, 219863910, 922622075) then user profile submitted (d_699625233) = yes (353358909)</t>
-  </si>
-  <si>
-    <t>If consent = yes then consent version = should be populated and be version 1 for their site (do one for each site). cross valid 2 rule. If consent = yes and site code = HP then they should have a consent version specific to their site (content should be specific to their site). Start out with rule for version just needing to be populated. Same for HIPAA. Later add rule for version 2 (0.02)</t>
-  </si>
-  <si>
-    <t>Edited rule for outreach required for manual verification- from line 25304 in https://nih.app.box.com/file/1153380782623</t>
-  </si>
-  <si>
-    <t>Edited rule for UP submitted line 30209 onwards in https://nih.app.box.com/file/1153380782623</t>
-  </si>
-  <si>
-    <t>Edited verification status rule from line 30484 in https://nih.app.box.com/file/1153380782623</t>
-  </si>
-  <si>
-    <t>Participant consent date d_982402227 (lines 30549-30696) Looks like this is a yyyymmdd format- This variable is deprecated. This rule can be removed entirely</t>
-  </si>
-  <si>
     <t>875007964, 219863910, 922622075, 160161595</t>
   </si>
   <si>
     <t>crossValid1 is not populated</t>
+  </si>
+  <si>
+    <t>If verification status (d_821247024) = verified (197316935) then sign in (d_230663853) = yes (353358909)</t>
+  </si>
+  <si>
+    <t>If verification status (d_821247024) = verified (197316935) then consented (d_919254129) = yes (353358909)</t>
+  </si>
+  <si>
+    <t>If verification status (d_821247024) = verified (197316935) then user profile submitted (d_699625233) = yes (353358909)</t>
   </si>
 </sst>
 </file>
@@ -2075,20 +2087,19 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2109,26 +2120,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFACFF9"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA9D8DE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB8F5D3"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCC7C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA9D8DE"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2218,29 +2217,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2665,531 +2662,24 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E4A111-52C2-714F-AC54-2C2FB898D55D}">
-  <dimension ref="A1:O21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="24.83203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="24.83203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>433</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>412</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="17">
-        <v>353358909</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>401</v>
-      </c>
-      <c r="D3" s="17">
-        <v>353358909</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>543</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="17">
-        <v>104430631</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>545</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="O5" s="17" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>547</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>548</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="17">
-        <v>104430631</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="O6" s="17" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>548</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="O7" s="17" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
-        <v>552</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="17">
-        <v>104430631</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="O8" s="17" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="O9" s="17" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>556</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="17">
-        <v>875007964</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="O10" s="17" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
-        <v>559</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>582</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>556</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>557</v>
-      </c>
-      <c r="O11" s="17" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>561</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="17">
-        <v>104430631</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>564</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="O13" s="17" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>566</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>567</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="F14" s="17">
-        <v>922622075</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="17">
-        <v>922622075</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>566</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>567</v>
-      </c>
-      <c r="O15" s="17" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>352</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>323</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="20">
-        <v>104430631</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="O16" s="20" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>543</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="21">
-        <v>353358909</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="F17" s="21">
-        <v>353358909</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
-        <v>547</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>548</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="21">
-        <v>353358909</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="F18" s="21">
-        <v>353358909</v>
-      </c>
-      <c r="O18" s="21" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="22">
-        <v>353358909</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="O19" s="22" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="22">
-        <v>353358909</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="O20" s="22" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
-        <v>552</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="22">
-        <v>353358909</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="O21" s="22" t="s">
-        <v>575</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="O2" dT="2023-04-14T18:26:19.03" personId="{2B6314D8-DBC2-0D44-8D0C-B73D0CA261B3}" id="{2BE77726-DB08-3448-8230-B667FCA9D175}">
+    <text>Need to add a crossvaligdation option for checking if the cross variable is a valid date in order to execute this rule</text>
+  </threadedComment>
+  <threadedComment ref="A3" dT="2023-04-14T19:16:02.66" personId="{2B6314D8-DBC2-0D44-8D0C-B73D0CA261B3}" id="{13F41FFA-F201-0240-B037-1C67A50FB39B}">
+    <text>These ones need a tweak to the code. “crossValid1 is not populated” rule should not flag participants for whom the ConceptID of interest is empty.</text>
+  </threadedComment>
+</ThreadedComments>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AFE071A-3C83-9E45-B616-577D581A90B9}">
-  <dimension ref="A1:Q189"/>
+  <dimension ref="A1:Q202"/>
   <sheetViews>
     <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6047,7 +5537,7 @@
       <c r="F129" s="1">
         <v>353358909</v>
       </c>
-      <c r="O129" s="26" t="s">
+      <c r="O129" s="21" t="s">
         <v>353</v>
       </c>
     </row>
@@ -7327,7 +6817,7 @@
         <v>36</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>16</v>
@@ -7378,7 +6868,7 @@
       <c r="C172" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="D172" s="25" t="s">
+      <c r="D172" s="20" t="s">
         <v>158</v>
       </c>
       <c r="E172" s="9" t="s">
@@ -7395,7 +6885,7 @@
       <c r="A173" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="B173" s="25" t="s">
+      <c r="B173" s="20" t="s">
         <v>158</v>
       </c>
       <c r="C173" s="9" t="s">
@@ -7684,7 +7174,7 @@
       <c r="A187" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="B187" s="25" t="s">
+      <c r="B187" s="20" t="s">
         <v>222</v>
       </c>
       <c r="C187" s="8" t="s">
@@ -7746,13 +7236,435 @@
       <c r="P188" s="8"/>
       <c r="Q188" s="8"/>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C189" s="25"/>
-      <c r="D189" s="27"/>
+    <row r="189" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="B189" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C189" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="E189" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F189" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="O189" s="27" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="27" t="s">
+        <v>543</v>
+      </c>
+      <c r="B190" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C190" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D190" s="27">
+        <v>104430631</v>
+      </c>
+      <c r="E190" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F190" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="O190" s="27" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="191" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="27" t="s">
+        <v>547</v>
+      </c>
+      <c r="B191" s="27" t="s">
+        <v>548</v>
+      </c>
+      <c r="C191" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D191" s="27">
+        <v>104430631</v>
+      </c>
+      <c r="E191" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="F191" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="O191" s="27" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="27" t="s">
+        <v>552</v>
+      </c>
+      <c r="B192" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="C192" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D192" s="27">
+        <v>104430631</v>
+      </c>
+      <c r="E192" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="F192" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="O192" s="27" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="B193" s="27" t="s">
+        <v>556</v>
+      </c>
+      <c r="C193" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D193" s="27">
+        <v>875007964</v>
+      </c>
+      <c r="E193" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="F193" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="O193" s="27" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="27" t="s">
+        <v>561</v>
+      </c>
+      <c r="B194" s="27" t="s">
+        <v>562</v>
+      </c>
+      <c r="C194" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D194" s="27">
+        <v>104430631</v>
+      </c>
+      <c r="E194" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F194" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="O194" s="27" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="B195" s="27" t="s">
+        <v>566</v>
+      </c>
+      <c r="C195" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D195" s="27" t="s">
+        <v>567</v>
+      </c>
+      <c r="E195" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="F195" s="27">
+        <v>922622075</v>
+      </c>
+      <c r="O195" s="27" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="B196" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="C196" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D196" s="27">
+        <v>922622075</v>
+      </c>
+      <c r="E196" s="27" t="s">
+        <v>566</v>
+      </c>
+      <c r="F196" s="27" t="s">
+        <v>567</v>
+      </c>
+      <c r="O196" s="27" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="B197" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="C197" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D197" s="27">
+        <v>104430631</v>
+      </c>
+      <c r="E197" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F197" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="O197" s="27" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="27" t="s">
+        <v>543</v>
+      </c>
+      <c r="B198" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C198" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D198" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E198" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="F198" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="O198" s="27" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="27" t="s">
+        <v>547</v>
+      </c>
+      <c r="B199" s="27" t="s">
+        <v>548</v>
+      </c>
+      <c r="C199" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D199" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E199" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="F199" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="O199" s="27" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="27" t="s">
+        <v>543</v>
+      </c>
+      <c r="B200" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C200" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D200" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E200" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="F200" s="27">
+        <v>197316935</v>
+      </c>
+      <c r="O200" s="27" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="27" t="s">
+        <v>547</v>
+      </c>
+      <c r="B201" s="27" t="s">
+        <v>548</v>
+      </c>
+      <c r="C201" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D201" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E201" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="F201" s="27">
+        <v>197316935</v>
+      </c>
+      <c r="O201" s="27" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="27" t="s">
+        <v>552</v>
+      </c>
+      <c r="B202" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="C202" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D202" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E202" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="F202" s="27">
+        <v>197316935</v>
+      </c>
+      <c r="O202" s="27" t="s">
+        <v>577</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E4A111-52C2-714F-AC54-2C2FB898D55D}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="20" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="142.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+    </row>
+    <row r="3" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8719,11 +8631,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3D455-1504-4B42-941B-931C7B0EFB28}">
-  <dimension ref="A1:O27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3D455-1504-4B42-941B-931C7B0EFB28}">
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8793,453 +8705,127 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>433</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" s="17">
+        <v>353358909</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="17">
-        <v>353358909</v>
-      </c>
       <c r="O2" s="17" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>72</v>
+        <v>545</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>401</v>
-      </c>
-      <c r="D3" s="17">
-        <v>353358909</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>78</v>
+        <v>574</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>378</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>543</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>261</v>
-      </c>
       <c r="O4" s="17" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>545</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>261</v>
+        <v>554</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>574</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>154</v>
+        <v>274</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>378</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>546</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>547</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>548</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>221</v>
+        <v>559</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>556</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>261</v>
+        <v>557</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>549</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>550</v>
+        <v>564</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>261</v>
+        <v>78</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>574</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>548</v>
+        <v>562</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>378</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
-        <v>552</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="O8" s="17" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="O9" s="17" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>556</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>557</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="O10" s="17" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
-        <v>559</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>556</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>557</v>
-      </c>
-      <c r="O11" s="17" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>561</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>564</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>562</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="O13" s="17" t="s">
         <v>565</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>566</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>567</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="F14" s="17">
-        <v>922622075</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="17">
-        <v>922622075</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>566</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>567</v>
-      </c>
-      <c r="O15" s="17" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>352</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>323</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>378</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="O16" s="20" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>543</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="21">
-        <v>353358909</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="F17" s="21">
-        <v>353358909</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
-        <v>547</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>548</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="21">
-        <v>353358909</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="F18" s="21">
-        <v>353358909</v>
-      </c>
-      <c r="O18" s="21" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="22">
-        <v>353358909</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="O19" s="22" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="22">
-        <v>353358909</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="O20" s="22" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
-        <v>552</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="22">
-        <v>353358909</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="O21" s="22" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="O22" s="1" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:15" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
-        <v>580</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set write_to_gcs to TRUE, modified gitignore
</commit_message>
<xml_diff>
--- a/qc_rules_recruitment.xlsx
+++ b/qc_rules_recruitment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersjm/Documents/qaqc_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DC51287-D54C-8A41-9EF1-DD5BC974E86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA5C287-ABF2-E448-9A92-D73950D4DECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
   </bookViews>
@@ -2681,8 +2681,8 @@
   <dimension ref="A1:Q202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O168" sqref="O168"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Issue #26: Removed "NA or" component of campaign type rules at 168-169
</commit_message>
<xml_diff>
--- a/qc_rules_recruitment.xlsx
+++ b/qc_rules_recruitment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersjm/Documents/qaqc_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D54C8-968A-AC40-9C0E-F6A2A6887CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1E41FD-9712-D14B-97C3-B461B75B05FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37580" yWindow="-3480" windowWidth="35920" windowHeight="17780" activeTab="6" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
+    <workbookView xWindow="3320" yWindow="1780" windowWidth="30240" windowHeight="17780" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
   </bookViews>
   <sheets>
     <sheet name="QAQC" sheetId="1" r:id="rId1"/>
@@ -2029,7 +2029,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2092,14 +2092,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2127,6 +2121,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2162,7 +2162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2224,13 +2224,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2238,6 +2231,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2677,9 +2673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AFE071A-3C83-9E45-B616-577D581A90B9}">
   <dimension ref="A1:Q202"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D205" sqref="D205"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6748,61 +6744,61 @@
         <v>377</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
+    <row r="168" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C168" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D168" s="1" t="s">
+      <c r="C168" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="D168" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E168" s="1" t="s">
+      <c r="E168" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F168" s="1">
+      <c r="F168" s="26">
         <v>486306141</v>
       </c>
-      <c r="M168" s="1" t="s">
+      <c r="M168" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="O168" s="1" t="s">
+      <c r="O168" s="26" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A169" s="1" t="s">
+    <row r="169" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C169" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D169" s="1" t="s">
+      <c r="C169" s="26" t="s">
+        <v>498</v>
+      </c>
+      <c r="D169" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E169" s="1" t="s">
+      <c r="E169" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F169" s="1">
+      <c r="F169" s="26">
         <v>854703046</v>
       </c>
-      <c r="G169" s="1" t="s">
+      <c r="G169" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="H169" s="1">
+      <c r="H169" s="26">
         <v>197316935</v>
       </c>
-      <c r="M169" s="1" t="s">
+      <c r="M169" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="O169" s="1" t="s">
+      <c r="O169" s="26" t="s">
         <v>377</v>
       </c>
     </row>
@@ -7236,322 +7232,322 @@
       <c r="P188" s="8"/>
       <c r="Q188" s="8"/>
     </row>
-    <row r="189" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="26" t="s">
+    <row r="189" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="B189" s="26" t="s">
+      <c r="B189" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C189" s="27" t="s">
+      <c r="C189" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="E189" s="27" t="s">
+      <c r="E189" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="F189" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="O189" s="27" t="s">
+      <c r="F189" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="O189" s="24" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="190" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="27" t="s">
+    <row r="190" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="B190" s="27" t="s">
+      <c r="B190" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C190" s="27" t="s">
+      <c r="C190" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D190" s="27">
+      <c r="D190" s="24">
         <v>104430631</v>
       </c>
-      <c r="E190" s="27" t="s">
+      <c r="E190" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="F190" s="27" t="s">
+      <c r="F190" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O190" s="27" t="s">
+      <c r="O190" s="24" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="191" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="27" t="s">
+    <row r="191" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="24" t="s">
         <v>547</v>
       </c>
-      <c r="B191" s="27" t="s">
+      <c r="B191" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="C191" s="27" t="s">
+      <c r="C191" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D191" s="27">
+      <c r="D191" s="24">
         <v>104430631</v>
       </c>
-      <c r="E191" s="28" t="s">
+      <c r="E191" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F191" s="27" t="s">
+      <c r="F191" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O191" s="27" t="s">
+      <c r="O191" s="24" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="27" t="s">
+    <row r="192" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="24" t="s">
         <v>552</v>
       </c>
-      <c r="B192" s="27" t="s">
+      <c r="B192" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="C192" s="27" t="s">
+      <c r="C192" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D192" s="27">
+      <c r="D192" s="24">
         <v>104430631</v>
       </c>
-      <c r="E192" s="28" t="s">
+      <c r="E192" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="F192" s="27" t="s">
+      <c r="F192" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O192" s="27" t="s">
+      <c r="O192" s="24" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="193" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="27" t="s">
+    <row r="193" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="B193" s="27" t="s">
+      <c r="B193" s="24" t="s">
         <v>556</v>
       </c>
-      <c r="C193" s="27" t="s">
+      <c r="C193" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D193" s="27">
+      <c r="D193" s="24">
         <v>875007964</v>
       </c>
-      <c r="E193" s="28" t="s">
+      <c r="E193" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="F193" s="27" t="s">
+      <c r="F193" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O193" s="27" t="s">
+      <c r="O193" s="24" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="194" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="27" t="s">
+    <row r="194" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="B194" s="27" t="s">
+      <c r="B194" s="24" t="s">
         <v>562</v>
       </c>
-      <c r="C194" s="27" t="s">
+      <c r="C194" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D194" s="27">
+      <c r="D194" s="24">
         <v>104430631</v>
       </c>
-      <c r="E194" s="28" t="s">
+      <c r="E194" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="F194" s="27" t="s">
+      <c r="F194" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O194" s="27" t="s">
+      <c r="O194" s="24" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="195" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="27" t="s">
+    <row r="195" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="24" t="s">
         <v>327</v>
       </c>
-      <c r="B195" s="27" t="s">
+      <c r="B195" s="24" t="s">
         <v>566</v>
       </c>
-      <c r="C195" s="27" t="s">
+      <c r="C195" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D195" s="27" t="s">
+      <c r="D195" s="24" t="s">
         <v>567</v>
       </c>
-      <c r="E195" s="27" t="s">
+      <c r="E195" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F195" s="27">
+      <c r="F195" s="24">
         <v>922622075</v>
       </c>
-      <c r="O195" s="27" t="s">
+      <c r="O195" s="24" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="196" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="27" t="s">
+    <row r="196" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="B196" s="27" t="s">
+      <c r="B196" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="C196" s="27" t="s">
+      <c r="C196" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D196" s="27">
+      <c r="D196" s="24">
         <v>922622075</v>
       </c>
-      <c r="E196" s="27" t="s">
+      <c r="E196" s="24" t="s">
         <v>566</v>
       </c>
-      <c r="F196" s="27" t="s">
+      <c r="F196" s="24" t="s">
         <v>567</v>
       </c>
-      <c r="O196" s="27" t="s">
+      <c r="O196" s="24" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="197" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="27" t="s">
+    <row r="197" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="24" t="s">
         <v>352</v>
       </c>
-      <c r="B197" s="27" t="s">
+      <c r="B197" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="C197" s="27" t="s">
+      <c r="C197" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D197" s="27">
+      <c r="D197" s="24">
         <v>104430631</v>
       </c>
-      <c r="E197" s="28" t="s">
+      <c r="E197" s="25" t="s">
         <v>326</v>
       </c>
-      <c r="F197" s="27" t="s">
+      <c r="F197" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="O197" s="27" t="s">
+      <c r="O197" s="24" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="198" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="27" t="s">
+    <row r="198" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="B198" s="27" t="s">
+      <c r="B198" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C198" s="27" t="s">
+      <c r="C198" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D198" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E198" s="27" t="s">
+      <c r="D198" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E198" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="F198" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="O198" s="27" t="s">
+      <c r="F198" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="O198" s="24" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="199" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A199" s="27" t="s">
+    <row r="199" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="24" t="s">
         <v>547</v>
       </c>
-      <c r="B199" s="27" t="s">
+      <c r="B199" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="C199" s="27" t="s">
+      <c r="C199" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D199" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E199" s="27" t="s">
+      <c r="D199" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E199" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="F199" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="O199" s="27" t="s">
+      <c r="F199" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="O199" s="24" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="200" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A200" s="27" t="s">
+    <row r="200" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="B200" s="27" t="s">
+      <c r="B200" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C200" s="27" t="s">
+      <c r="C200" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D200" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E200" s="27" t="s">
+      <c r="D200" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E200" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F200" s="27">
+      <c r="F200" s="24">
         <v>197316935</v>
       </c>
-      <c r="O200" s="27" t="s">
+      <c r="O200" s="24" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="201" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A201" s="27" t="s">
+    <row r="201" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="24" t="s">
         <v>547</v>
       </c>
-      <c r="B201" s="27" t="s">
+      <c r="B201" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="C201" s="27" t="s">
+      <c r="C201" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D201" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E201" s="27" t="s">
+      <c r="D201" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E201" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F201" s="27">
+      <c r="F201" s="24">
         <v>197316935</v>
       </c>
-      <c r="O201" s="27" t="s">
+      <c r="O201" s="24" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="202" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="27" t="s">
+    <row r="202" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="24" t="s">
         <v>552</v>
       </c>
-      <c r="B202" s="27" t="s">
+      <c r="B202" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="C202" s="27" t="s">
+      <c r="C202" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D202" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E202" s="27" t="s">
+      <c r="D202" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E202" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F202" s="27">
+      <c r="F202" s="24">
         <v>197316935</v>
       </c>
-      <c r="O202" s="27" t="s">
+      <c r="O202" s="24" t="s">
         <v>577</v>
       </c>
     </row>
@@ -7635,33 +7631,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-    </row>
-    <row r="3" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E5" s="25"/>
-    </row>
-    <row r="6" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8634,7 +8630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3D455-1504-4B42-941B-931C7B0EFB28}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert "Issue #26: Removed "NA or" component of campaign type rules at 168-169"
</commit_message>
<xml_diff>
--- a/qc_rules_recruitment.xlsx
+++ b/qc_rules_recruitment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersjm/Documents/qaqc_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1E41FD-9712-D14B-97C3-B461B75B05FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D54C8-968A-AC40-9C0E-F6A2A6887CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="1780" windowWidth="30240" windowHeight="17780" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
+    <workbookView xWindow="-37580" yWindow="-3480" windowWidth="35920" windowHeight="17780" activeTab="6" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
   </bookViews>
   <sheets>
     <sheet name="QAQC" sheetId="1" r:id="rId1"/>
@@ -2029,7 +2029,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2092,8 +2092,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2121,12 +2127,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2162,7 +2162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2224,6 +2224,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2231,9 +2238,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2673,9 +2677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AFE071A-3C83-9E45-B616-577D581A90B9}">
   <dimension ref="A1:Q202"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C169" sqref="C169"/>
+    <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6744,61 +6748,61 @@
         <v>377</v>
       </c>
     </row>
-    <row r="168" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="26" t="s">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B168" s="26" t="s">
+      <c r="B168" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C168" s="26" t="s">
-        <v>495</v>
-      </c>
-      <c r="D168" s="26" t="s">
+      <c r="C168" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E168" s="26" t="s">
+      <c r="E168" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F168" s="26">
+      <c r="F168" s="1">
         <v>486306141</v>
       </c>
-      <c r="M168" s="26" t="s">
+      <c r="M168" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O168" s="26" t="s">
+      <c r="O168" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="169" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="26" t="s">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B169" s="26" t="s">
+      <c r="B169" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C169" s="26" t="s">
-        <v>498</v>
-      </c>
-      <c r="D169" s="26" t="s">
+      <c r="C169" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D169" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E169" s="26" t="s">
+      <c r="E169" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F169" s="26">
+      <c r="F169" s="1">
         <v>854703046</v>
       </c>
-      <c r="G169" s="26" t="s">
+      <c r="G169" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="H169" s="26">
+      <c r="H169" s="1">
         <v>197316935</v>
       </c>
-      <c r="M169" s="26" t="s">
+      <c r="M169" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O169" s="26" t="s">
+      <c r="O169" s="1" t="s">
         <v>377</v>
       </c>
     </row>
@@ -7232,322 +7236,322 @@
       <c r="P188" s="8"/>
       <c r="Q188" s="8"/>
     </row>
-    <row r="189" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="23" t="s">
+    <row r="189" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="26" t="s">
         <v>433</v>
       </c>
-      <c r="B189" s="23" t="s">
+      <c r="B189" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C189" s="24" t="s">
+      <c r="C189" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="E189" s="24" t="s">
+      <c r="E189" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F189" s="24">
-        <v>353358909</v>
-      </c>
-      <c r="O189" s="24" t="s">
+      <c r="F189" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="O189" s="27" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="190" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="24" t="s">
+    <row r="190" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="27" t="s">
         <v>543</v>
       </c>
-      <c r="B190" s="24" t="s">
+      <c r="B190" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="C190" s="24" t="s">
+      <c r="C190" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D190" s="24">
+      <c r="D190" s="27">
         <v>104430631</v>
       </c>
-      <c r="E190" s="24" t="s">
+      <c r="E190" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="F190" s="24" t="s">
+      <c r="F190" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="O190" s="24" t="s">
+      <c r="O190" s="27" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="191" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="24" t="s">
+    <row r="191" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="27" t="s">
         <v>547</v>
       </c>
-      <c r="B191" s="24" t="s">
+      <c r="B191" s="27" t="s">
         <v>548</v>
       </c>
-      <c r="C191" s="24" t="s">
+      <c r="C191" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D191" s="24">
+      <c r="D191" s="27">
         <v>104430631</v>
       </c>
-      <c r="E191" s="25" t="s">
+      <c r="E191" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="F191" s="24" t="s">
+      <c r="F191" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="O191" s="24" t="s">
+      <c r="O191" s="27" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="24" t="s">
+    <row r="192" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="27" t="s">
         <v>552</v>
       </c>
-      <c r="B192" s="24" t="s">
+      <c r="B192" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="C192" s="24" t="s">
+      <c r="C192" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D192" s="24">
+      <c r="D192" s="27">
         <v>104430631</v>
       </c>
-      <c r="E192" s="25" t="s">
+      <c r="E192" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="F192" s="24" t="s">
+      <c r="F192" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="O192" s="24" t="s">
+      <c r="O192" s="27" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="193" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="24" t="s">
+    <row r="193" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="B193" s="24" t="s">
+      <c r="B193" s="27" t="s">
         <v>556</v>
       </c>
-      <c r="C193" s="24" t="s">
+      <c r="C193" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D193" s="24">
+      <c r="D193" s="27">
         <v>875007964</v>
       </c>
-      <c r="E193" s="25" t="s">
+      <c r="E193" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="F193" s="24" t="s">
+      <c r="F193" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="O193" s="24" t="s">
+      <c r="O193" s="27" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="194" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="24" t="s">
+    <row r="194" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="27" t="s">
         <v>561</v>
       </c>
-      <c r="B194" s="24" t="s">
+      <c r="B194" s="27" t="s">
         <v>562</v>
       </c>
-      <c r="C194" s="24" t="s">
+      <c r="C194" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D194" s="24">
+      <c r="D194" s="27">
         <v>104430631</v>
       </c>
-      <c r="E194" s="25" t="s">
+      <c r="E194" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F194" s="24" t="s">
+      <c r="F194" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="O194" s="24" t="s">
+      <c r="O194" s="27" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="195" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="24" t="s">
+    <row r="195" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="27" t="s">
         <v>327</v>
       </c>
-      <c r="B195" s="24" t="s">
+      <c r="B195" s="27" t="s">
         <v>566</v>
       </c>
-      <c r="C195" s="24" t="s">
+      <c r="C195" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D195" s="24" t="s">
+      <c r="D195" s="27" t="s">
         <v>567</v>
       </c>
-      <c r="E195" s="24" t="s">
+      <c r="E195" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="F195" s="24">
+      <c r="F195" s="27">
         <v>922622075</v>
       </c>
-      <c r="O195" s="24" t="s">
+      <c r="O195" s="27" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="196" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="24" t="s">
+    <row r="196" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="B196" s="24" t="s">
+      <c r="B196" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="C196" s="24" t="s">
+      <c r="C196" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D196" s="24">
+      <c r="D196" s="27">
         <v>922622075</v>
       </c>
-      <c r="E196" s="24" t="s">
+      <c r="E196" s="27" t="s">
         <v>566</v>
       </c>
-      <c r="F196" s="24" t="s">
+      <c r="F196" s="27" t="s">
         <v>567</v>
       </c>
-      <c r="O196" s="24" t="s">
+      <c r="O196" s="27" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="197" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="24" t="s">
+    <row r="197" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="B197" s="24" t="s">
+      <c r="B197" s="27" t="s">
         <v>323</v>
       </c>
-      <c r="C197" s="24" t="s">
+      <c r="C197" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D197" s="24">
+      <c r="D197" s="27">
         <v>104430631</v>
       </c>
-      <c r="E197" s="25" t="s">
+      <c r="E197" s="28" t="s">
         <v>326</v>
       </c>
-      <c r="F197" s="24" t="s">
+      <c r="F197" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="O197" s="24" t="s">
+      <c r="O197" s="27" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="198" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="24" t="s">
+    <row r="198" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="27" t="s">
         <v>543</v>
       </c>
-      <c r="B198" s="24" t="s">
+      <c r="B198" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="C198" s="24" t="s">
+      <c r="C198" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D198" s="24">
-        <v>353358909</v>
-      </c>
-      <c r="E198" s="24" t="s">
+      <c r="D198" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E198" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="F198" s="24">
-        <v>353358909</v>
-      </c>
-      <c r="O198" s="24" t="s">
+      <c r="F198" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="O198" s="27" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="199" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A199" s="24" t="s">
+    <row r="199" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="27" t="s">
         <v>547</v>
       </c>
-      <c r="B199" s="24" t="s">
+      <c r="B199" s="27" t="s">
         <v>548</v>
       </c>
-      <c r="C199" s="24" t="s">
+      <c r="C199" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D199" s="24">
-        <v>353358909</v>
-      </c>
-      <c r="E199" s="24" t="s">
+      <c r="D199" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E199" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="F199" s="24">
-        <v>353358909</v>
-      </c>
-      <c r="O199" s="24" t="s">
+      <c r="F199" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="O199" s="27" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="200" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A200" s="24" t="s">
+    <row r="200" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="27" t="s">
         <v>543</v>
       </c>
-      <c r="B200" s="24" t="s">
+      <c r="B200" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="C200" s="24" t="s">
+      <c r="C200" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D200" s="24">
-        <v>353358909</v>
-      </c>
-      <c r="E200" s="24" t="s">
+      <c r="D200" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E200" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="F200" s="24">
+      <c r="F200" s="27">
         <v>197316935</v>
       </c>
-      <c r="O200" s="24" t="s">
+      <c r="O200" s="27" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="201" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A201" s="24" t="s">
+    <row r="201" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="27" t="s">
         <v>547</v>
       </c>
-      <c r="B201" s="24" t="s">
+      <c r="B201" s="27" t="s">
         <v>548</v>
       </c>
-      <c r="C201" s="24" t="s">
+      <c r="C201" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D201" s="24">
-        <v>353358909</v>
-      </c>
-      <c r="E201" s="24" t="s">
+      <c r="D201" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E201" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="F201" s="24">
+      <c r="F201" s="27">
         <v>197316935</v>
       </c>
-      <c r="O201" s="24" t="s">
+      <c r="O201" s="27" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="202" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="24" t="s">
+    <row r="202" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="27" t="s">
         <v>552</v>
       </c>
-      <c r="B202" s="24" t="s">
+      <c r="B202" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="C202" s="24" t="s">
+      <c r="C202" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D202" s="24">
-        <v>353358909</v>
-      </c>
-      <c r="E202" s="24" t="s">
+      <c r="D202" s="27">
+        <v>353358909</v>
+      </c>
+      <c r="E202" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="F202" s="24">
+      <c r="F202" s="27">
         <v>197316935</v>
       </c>
-      <c r="O202" s="24" t="s">
+      <c r="O202" s="27" t="s">
         <v>577</v>
       </c>
     </row>
@@ -7631,33 +7635,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E7" s="20"/>
-    </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E10" s="20"/>
-    </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+    </row>
+    <row r="3" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8630,7 +8634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3D455-1504-4B42-941B-931C7B0EFB28}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
"Issue #26: Removed "NA or " component of Campaign Type rules at 168,169
</commit_message>
<xml_diff>
--- a/qc_rules_recruitment.xlsx
+++ b/qc_rules_recruitment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersjm/Documents/qaqc_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D54C8-968A-AC40-9C0E-F6A2A6887CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40E8BAF-23B8-9648-8A81-F9443546D137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37580" yWindow="-3480" windowWidth="35920" windowHeight="17780" activeTab="6" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19580" xr2:uid="{8AC44F3B-8D47-B14A-85C0-6B36B0621E92}"/>
   </bookViews>
   <sheets>
     <sheet name="QAQC" sheetId="1" r:id="rId1"/>
@@ -2029,7 +2029,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2091,12 +2091,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2162,7 +2156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2224,13 +2218,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2677,9 +2664,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AFE071A-3C83-9E45-B616-577D581A90B9}">
   <dimension ref="A1:Q202"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D205" sqref="D205"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6756,7 +6743,7 @@
         <v>66</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>36</v>
+        <v>495</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>67</v>
@@ -6782,7 +6769,7 @@
         <v>66</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>354</v>
+        <v>498</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>67</v>
@@ -7236,322 +7223,322 @@
       <c r="P188" s="8"/>
       <c r="Q188" s="8"/>
     </row>
-    <row r="189" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="26" t="s">
+    <row r="189" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="B189" s="26" t="s">
+      <c r="B189" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C189" s="27" t="s">
+      <c r="C189" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="E189" s="27" t="s">
+      <c r="E189" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="F189" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="O189" s="27" t="s">
+      <c r="F189" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="O189" s="24" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="190" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="27" t="s">
+    <row r="190" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="B190" s="27" t="s">
+      <c r="B190" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C190" s="27" t="s">
+      <c r="C190" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D190" s="27">
+      <c r="D190" s="24">
         <v>104430631</v>
       </c>
-      <c r="E190" s="27" t="s">
+      <c r="E190" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="F190" s="27" t="s">
+      <c r="F190" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O190" s="27" t="s">
+      <c r="O190" s="24" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="191" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="27" t="s">
+    <row r="191" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="24" t="s">
         <v>547</v>
       </c>
-      <c r="B191" s="27" t="s">
+      <c r="B191" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="C191" s="27" t="s">
+      <c r="C191" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D191" s="27">
+      <c r="D191" s="24">
         <v>104430631</v>
       </c>
-      <c r="E191" s="28" t="s">
+      <c r="E191" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F191" s="27" t="s">
+      <c r="F191" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O191" s="27" t="s">
+      <c r="O191" s="24" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="27" t="s">
+    <row r="192" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="24" t="s">
         <v>552</v>
       </c>
-      <c r="B192" s="27" t="s">
+      <c r="B192" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="C192" s="27" t="s">
+      <c r="C192" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D192" s="27">
+      <c r="D192" s="24">
         <v>104430631</v>
       </c>
-      <c r="E192" s="28" t="s">
+      <c r="E192" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="F192" s="27" t="s">
+      <c r="F192" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O192" s="27" t="s">
+      <c r="O192" s="24" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="193" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="27" t="s">
+    <row r="193" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="B193" s="27" t="s">
+      <c r="B193" s="24" t="s">
         <v>556</v>
       </c>
-      <c r="C193" s="27" t="s">
+      <c r="C193" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D193" s="27">
+      <c r="D193" s="24">
         <v>875007964</v>
       </c>
-      <c r="E193" s="28" t="s">
+      <c r="E193" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="F193" s="27" t="s">
+      <c r="F193" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O193" s="27" t="s">
+      <c r="O193" s="24" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="194" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="27" t="s">
+    <row r="194" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="B194" s="27" t="s">
+      <c r="B194" s="24" t="s">
         <v>562</v>
       </c>
-      <c r="C194" s="27" t="s">
+      <c r="C194" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D194" s="27">
+      <c r="D194" s="24">
         <v>104430631</v>
       </c>
-      <c r="E194" s="28" t="s">
+      <c r="E194" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="F194" s="27" t="s">
+      <c r="F194" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="O194" s="27" t="s">
+      <c r="O194" s="24" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="195" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="27" t="s">
+    <row r="195" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="24" t="s">
         <v>327</v>
       </c>
-      <c r="B195" s="27" t="s">
+      <c r="B195" s="24" t="s">
         <v>566</v>
       </c>
-      <c r="C195" s="27" t="s">
+      <c r="C195" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D195" s="27" t="s">
+      <c r="D195" s="24" t="s">
         <v>567</v>
       </c>
-      <c r="E195" s="27" t="s">
+      <c r="E195" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F195" s="27">
+      <c r="F195" s="24">
         <v>922622075</v>
       </c>
-      <c r="O195" s="27" t="s">
+      <c r="O195" s="24" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="196" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="27" t="s">
+    <row r="196" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="B196" s="27" t="s">
+      <c r="B196" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="C196" s="27" t="s">
+      <c r="C196" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D196" s="27">
+      <c r="D196" s="24">
         <v>922622075</v>
       </c>
-      <c r="E196" s="27" t="s">
+      <c r="E196" s="24" t="s">
         <v>566</v>
       </c>
-      <c r="F196" s="27" t="s">
+      <c r="F196" s="24" t="s">
         <v>567</v>
       </c>
-      <c r="O196" s="27" t="s">
+      <c r="O196" s="24" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="197" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="27" t="s">
+    <row r="197" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="24" t="s">
         <v>352</v>
       </c>
-      <c r="B197" s="27" t="s">
+      <c r="B197" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="C197" s="27" t="s">
+      <c r="C197" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D197" s="27">
+      <c r="D197" s="24">
         <v>104430631</v>
       </c>
-      <c r="E197" s="28" t="s">
+      <c r="E197" s="25" t="s">
         <v>326</v>
       </c>
-      <c r="F197" s="27" t="s">
+      <c r="F197" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="O197" s="27" t="s">
+      <c r="O197" s="24" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="198" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="27" t="s">
+    <row r="198" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="B198" s="27" t="s">
+      <c r="B198" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C198" s="27" t="s">
+      <c r="C198" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D198" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E198" s="27" t="s">
+      <c r="D198" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E198" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="F198" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="O198" s="27" t="s">
+      <c r="F198" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="O198" s="24" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="199" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A199" s="27" t="s">
+    <row r="199" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="24" t="s">
         <v>547</v>
       </c>
-      <c r="B199" s="27" t="s">
+      <c r="B199" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="C199" s="27" t="s">
+      <c r="C199" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D199" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E199" s="27" t="s">
+      <c r="D199" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E199" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="F199" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="O199" s="27" t="s">
+      <c r="F199" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="O199" s="24" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="200" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A200" s="27" t="s">
+    <row r="200" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="B200" s="27" t="s">
+      <c r="B200" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C200" s="27" t="s">
+      <c r="C200" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D200" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E200" s="27" t="s">
+      <c r="D200" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E200" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F200" s="27">
+      <c r="F200" s="24">
         <v>197316935</v>
       </c>
-      <c r="O200" s="27" t="s">
+      <c r="O200" s="24" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="201" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A201" s="27" t="s">
+    <row r="201" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="24" t="s">
         <v>547</v>
       </c>
-      <c r="B201" s="27" t="s">
+      <c r="B201" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="C201" s="27" t="s">
+      <c r="C201" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D201" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E201" s="27" t="s">
+      <c r="D201" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E201" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F201" s="27">
+      <c r="F201" s="24">
         <v>197316935</v>
       </c>
-      <c r="O201" s="27" t="s">
+      <c r="O201" s="24" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="202" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="27" t="s">
+    <row r="202" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="24" t="s">
         <v>552</v>
       </c>
-      <c r="B202" s="27" t="s">
+      <c r="B202" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="C202" s="27" t="s">
+      <c r="C202" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D202" s="27">
-        <v>353358909</v>
-      </c>
-      <c r="E202" s="27" t="s">
+      <c r="D202" s="24">
+        <v>353358909</v>
+      </c>
+      <c r="E202" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F202" s="27">
+      <c r="F202" s="24">
         <v>197316935</v>
       </c>
-      <c r="O202" s="27" t="s">
+      <c r="O202" s="24" t="s">
         <v>577</v>
       </c>
     </row>
@@ -7635,33 +7622,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-    </row>
-    <row r="3" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E5" s="25"/>
-    </row>
-    <row r="6" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:15" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8634,7 +8621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B3D455-1504-4B42-941B-931C7B0EFB28}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>